<commit_message>
Working Header and Betslip
</commit_message>
<xml_diff>
--- a/src/global/utils/file-utils/locators(1).xlsx
+++ b/src/global/utils/file-utils/locators(1).xlsx
@@ -1589,6 +1589,9 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="10" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1615,9 +1618,6 @@
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="14" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1971,7 +1971,7 @@
       <c r="D2" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="32" t="s">
+      <c r="E2" s="23" t="s">
         <v>415</v>
       </c>
       <c r="F2" s="13">
@@ -1991,7 +1991,7 @@
       <c r="D3" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="32" t="s">
+      <c r="E3" s="23" t="s">
         <v>417</v>
       </c>
       <c r="F3" s="13"/>
@@ -2009,7 +2009,7 @@
       <c r="D4" s="11" t="s">
         <v>419</v>
       </c>
-      <c r="E4" s="32" t="s">
+      <c r="E4" s="23" t="s">
         <v>19</v>
       </c>
       <c r="F4" s="13"/>
@@ -2027,7 +2027,7 @@
       <c r="D5" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="32" t="s">
+      <c r="E5" s="23" t="s">
         <v>421</v>
       </c>
       <c r="F5" s="13"/>
@@ -2045,7 +2045,7 @@
       <c r="D6" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="32" t="s">
+      <c r="E6" s="23" t="s">
         <v>423</v>
       </c>
       <c r="F6" s="13"/>
@@ -2063,7 +2063,7 @@
       <c r="D7" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="32" t="s">
+      <c r="E7" s="23" t="s">
         <v>425</v>
       </c>
       <c r="F7" s="13"/>
@@ -2081,7 +2081,7 @@
       <c r="D8" s="11" t="s">
         <v>427</v>
       </c>
-      <c r="E8" s="32" t="s">
+      <c r="E8" s="23" t="s">
         <v>19</v>
       </c>
       <c r="F8" s="13"/>
@@ -2099,7 +2099,7 @@
       <c r="D9" s="11" t="s">
         <v>429</v>
       </c>
-      <c r="E9" s="32" t="s">
+      <c r="E9" s="23" t="s">
         <v>19</v>
       </c>
       <c r="F9" s="13"/>
@@ -2117,7 +2117,7 @@
       <c r="D10" s="11" t="s">
         <v>431</v>
       </c>
-      <c r="E10" s="32" t="s">
+      <c r="E10" s="23" t="s">
         <v>19</v>
       </c>
       <c r="F10" s="13"/>
@@ -2135,7 +2135,7 @@
       <c r="D11" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="32" t="s">
+      <c r="E11" s="23" t="s">
         <v>433</v>
       </c>
       <c r="F11" s="13"/>
@@ -2153,7 +2153,7 @@
       <c r="D12" s="11" t="s">
         <v>435</v>
       </c>
-      <c r="E12" s="32" t="s">
+      <c r="E12" s="23" t="s">
         <v>19</v>
       </c>
       <c r="F12" s="13"/>
@@ -2171,7 +2171,7 @@
       <c r="D13" s="11" t="s">
         <v>436</v>
       </c>
-      <c r="E13" s="32" t="s">
+      <c r="E13" s="23" t="s">
         <v>19</v>
       </c>
       <c r="F13" s="13"/>
@@ -2189,7 +2189,7 @@
       <c r="D14" s="11" t="s">
         <v>438</v>
       </c>
-      <c r="E14" s="32" t="s">
+      <c r="E14" s="23" t="s">
         <v>19</v>
       </c>
       <c r="F14" s="13"/>
@@ -2207,7 +2207,7 @@
       <c r="D15" s="11" t="s">
         <v>440</v>
       </c>
-      <c r="E15" s="32" t="s">
+      <c r="E15" s="23" t="s">
         <v>19</v>
       </c>
       <c r="F15" s="13"/>
@@ -2225,7 +2225,7 @@
       <c r="D16" s="11" t="s">
         <v>442</v>
       </c>
-      <c r="E16" s="32" t="s">
+      <c r="E16" s="23" t="s">
         <v>19</v>
       </c>
       <c r="F16" s="13"/>
@@ -2243,7 +2243,7 @@
       <c r="D17" s="11" t="s">
         <v>444</v>
       </c>
-      <c r="E17" s="32" t="s">
+      <c r="E17" s="23" t="s">
         <v>19</v>
       </c>
       <c r="F17" s="13"/>
@@ -2261,7 +2261,7 @@
       <c r="D18" s="11" t="s">
         <v>446</v>
       </c>
-      <c r="E18" s="32" t="s">
+      <c r="E18" s="23" t="s">
         <v>19</v>
       </c>
       <c r="F18" s="13"/>
@@ -2279,7 +2279,7 @@
       <c r="D19" s="33" t="s">
         <v>448</v>
       </c>
-      <c r="E19" s="32" t="s">
+      <c r="E19" s="23" t="s">
         <v>19</v>
       </c>
       <c r="F19" s="13"/>
@@ -2289,7 +2289,7 @@
       <c r="B20" s="11"/>
       <c r="C20" s="11"/>
       <c r="D20" s="11"/>
-      <c r="E20" s="32"/>
+      <c r="E20" s="23"/>
       <c r="F20" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
@@ -2297,7 +2297,7 @@
       <c r="B21" s="11"/>
       <c r="C21" s="11"/>
       <c r="D21" s="11"/>
-      <c r="E21" s="32"/>
+      <c r="E21" s="23"/>
       <c r="F21" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
@@ -2305,7 +2305,7 @@
       <c r="B22" s="11"/>
       <c r="C22" s="11"/>
       <c r="D22" s="11"/>
-      <c r="E22" s="32"/>
+      <c r="E22" s="23"/>
       <c r="F22" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
@@ -2313,7 +2313,7 @@
       <c r="B23" s="11"/>
       <c r="C23" s="11"/>
       <c r="D23" s="11"/>
-      <c r="E23" s="32"/>
+      <c r="E23" s="23"/>
       <c r="F23" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
@@ -2321,7 +2321,7 @@
       <c r="B24" s="11"/>
       <c r="C24" s="11"/>
       <c r="D24" s="11"/>
-      <c r="E24" s="32"/>
+      <c r="E24" s="23"/>
       <c r="F24" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
@@ -2329,7 +2329,7 @@
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
       <c r="D25" s="11"/>
-      <c r="E25" s="32"/>
+      <c r="E25" s="23"/>
       <c r="F25" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
@@ -2337,7 +2337,7 @@
       <c r="B26" s="11"/>
       <c r="C26" s="11"/>
       <c r="D26" s="11"/>
-      <c r="E26" s="32"/>
+      <c r="E26" s="23"/>
       <c r="F26" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
@@ -2345,7 +2345,7 @@
       <c r="B27" s="11"/>
       <c r="C27" s="11"/>
       <c r="D27" s="11"/>
-      <c r="E27" s="32"/>
+      <c r="E27" s="23"/>
       <c r="F27" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
@@ -2353,7 +2353,7 @@
       <c r="B28" s="11"/>
       <c r="C28" s="11"/>
       <c r="D28" s="11"/>
-      <c r="E28" s="32"/>
+      <c r="E28" s="23"/>
       <c r="F28" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
@@ -2361,7 +2361,7 @@
       <c r="B29" s="11"/>
       <c r="C29" s="11"/>
       <c r="D29" s="11"/>
-      <c r="E29" s="32"/>
+      <c r="E29" s="23"/>
       <c r="F29" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
@@ -2369,7 +2369,7 @@
       <c r="B30" s="11"/>
       <c r="C30" s="11"/>
       <c r="D30" s="11"/>
-      <c r="E30" s="32"/>
+      <c r="E30" s="23"/>
       <c r="F30" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
@@ -2377,7 +2377,7 @@
       <c r="B31" s="11"/>
       <c r="C31" s="11"/>
       <c r="D31" s="11"/>
-      <c r="E31" s="32"/>
+      <c r="E31" s="23"/>
       <c r="F31" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
@@ -2385,7 +2385,7 @@
       <c r="B32" s="11"/>
       <c r="C32" s="11"/>
       <c r="D32" s="11"/>
-      <c r="E32" s="32"/>
+      <c r="E32" s="23"/>
       <c r="F32" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
@@ -2393,7 +2393,7 @@
       <c r="B33" s="11"/>
       <c r="C33" s="11"/>
       <c r="D33" s="11"/>
-      <c r="E33" s="32"/>
+      <c r="E33" s="23"/>
       <c r="F33" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
@@ -2401,7 +2401,7 @@
       <c r="B34" s="11"/>
       <c r="C34" s="11"/>
       <c r="D34" s="11"/>
-      <c r="E34" s="32"/>
+      <c r="E34" s="23"/>
       <c r="F34" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
@@ -2409,7 +2409,7 @@
       <c r="B35" s="11"/>
       <c r="C35" s="11"/>
       <c r="D35" s="11"/>
-      <c r="E35" s="32"/>
+      <c r="E35" s="23"/>
       <c r="F35" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
@@ -2417,7 +2417,7 @@
       <c r="B36" s="11"/>
       <c r="C36" s="11"/>
       <c r="D36" s="11"/>
-      <c r="E36" s="32"/>
+      <c r="E36" s="23"/>
       <c r="F36" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
@@ -2425,7 +2425,7 @@
       <c r="B37" s="11"/>
       <c r="C37" s="11"/>
       <c r="D37" s="11"/>
-      <c r="E37" s="32"/>
+      <c r="E37" s="23"/>
       <c r="F37" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
@@ -2433,7 +2433,7 @@
       <c r="B38" s="11"/>
       <c r="C38" s="11"/>
       <c r="D38" s="11"/>
-      <c r="E38" s="32"/>
+      <c r="E38" s="23"/>
       <c r="F38" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
@@ -2441,7 +2441,7 @@
       <c r="B39" s="11"/>
       <c r="C39" s="11"/>
       <c r="D39" s="11"/>
-      <c r="E39" s="32"/>
+      <c r="E39" s="23"/>
       <c r="F39" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
@@ -2449,7 +2449,7 @@
       <c r="B40" s="11"/>
       <c r="C40" s="11"/>
       <c r="D40" s="11"/>
-      <c r="E40" s="32"/>
+      <c r="E40" s="23"/>
       <c r="F40" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
@@ -2457,7 +2457,7 @@
       <c r="B41" s="11"/>
       <c r="C41" s="11"/>
       <c r="D41" s="11"/>
-      <c r="E41" s="32"/>
+      <c r="E41" s="23"/>
       <c r="F41" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
@@ -2465,7 +2465,7 @@
       <c r="B42" s="11"/>
       <c r="C42" s="11"/>
       <c r="D42" s="11"/>
-      <c r="E42" s="32"/>
+      <c r="E42" s="23"/>
       <c r="F42" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
@@ -2473,7 +2473,7 @@
       <c r="B43" s="11"/>
       <c r="C43" s="11"/>
       <c r="D43" s="11"/>
-      <c r="E43" s="32"/>
+      <c r="E43" s="23"/>
       <c r="F43" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
@@ -2481,7 +2481,7 @@
       <c r="B44" s="11"/>
       <c r="C44" s="11"/>
       <c r="D44" s="11"/>
-      <c r="E44" s="32"/>
+      <c r="E44" s="23"/>
       <c r="F44" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
@@ -2489,7 +2489,7 @@
       <c r="B45" s="11"/>
       <c r="C45" s="11"/>
       <c r="D45" s="11"/>
-      <c r="E45" s="32"/>
+      <c r="E45" s="23"/>
       <c r="F45" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
@@ -2497,7 +2497,7 @@
       <c r="B46" s="11"/>
       <c r="C46" s="11"/>
       <c r="D46" s="11"/>
-      <c r="E46" s="32"/>
+      <c r="E46" s="23"/>
       <c r="F46" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
@@ -2505,7 +2505,7 @@
       <c r="B47" s="11"/>
       <c r="C47" s="11"/>
       <c r="D47" s="11"/>
-      <c r="E47" s="32"/>
+      <c r="E47" s="23"/>
       <c r="F47" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
@@ -2513,7 +2513,7 @@
       <c r="B48" s="11"/>
       <c r="C48" s="11"/>
       <c r="D48" s="11"/>
-      <c r="E48" s="32"/>
+      <c r="E48" s="23"/>
       <c r="F48" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
@@ -2521,7 +2521,7 @@
       <c r="B49" s="11"/>
       <c r="C49" s="11"/>
       <c r="D49" s="11"/>
-      <c r="E49" s="32"/>
+      <c r="E49" s="23"/>
       <c r="F49" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
@@ -2649,7 +2649,7 @@
       <c r="B65" s="11"/>
       <c r="C65" s="11"/>
       <c r="D65" s="11"/>
-      <c r="E65" s="32"/>
+      <c r="E65" s="23"/>
       <c r="F65" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18.75">
@@ -2809,7 +2809,7 @@
       <c r="B85" s="11"/>
       <c r="C85" s="11"/>
       <c r="D85" s="11"/>
-      <c r="E85" s="32"/>
+      <c r="E85" s="23"/>
       <c r="F85" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="18.75">
@@ -2817,7 +2817,7 @@
       <c r="B86" s="11"/>
       <c r="C86" s="11"/>
       <c r="D86" s="11"/>
-      <c r="E86" s="32"/>
+      <c r="E86" s="23"/>
       <c r="F86" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="18.75">
@@ -2825,7 +2825,7 @@
       <c r="B87" s="11"/>
       <c r="C87" s="11"/>
       <c r="D87" s="11"/>
-      <c r="E87" s="32"/>
+      <c r="E87" s="23"/>
       <c r="F87" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="18.75">
@@ -2833,7 +2833,7 @@
       <c r="B88" s="11"/>
       <c r="C88" s="11"/>
       <c r="D88" s="11"/>
-      <c r="E88" s="32"/>
+      <c r="E88" s="23"/>
       <c r="F88" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="18.75">
@@ -2841,7 +2841,7 @@
       <c r="B89" s="11"/>
       <c r="C89" s="11"/>
       <c r="D89" s="11"/>
-      <c r="E89" s="32"/>
+      <c r="E89" s="23"/>
       <c r="F89" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="18.75">
@@ -2849,7 +2849,7 @@
       <c r="B90" s="11"/>
       <c r="C90" s="11"/>
       <c r="D90" s="11"/>
-      <c r="E90" s="32"/>
+      <c r="E90" s="23"/>
       <c r="F90" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="18.75">
@@ -2857,7 +2857,7 @@
       <c r="B91" s="11"/>
       <c r="C91" s="11"/>
       <c r="D91" s="11"/>
-      <c r="E91" s="32"/>
+      <c r="E91" s="23"/>
       <c r="F91" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="18.75">
@@ -2865,7 +2865,7 @@
       <c r="B92" s="11"/>
       <c r="C92" s="11"/>
       <c r="D92" s="11"/>
-      <c r="E92" s="32"/>
+      <c r="E92" s="23"/>
       <c r="F92" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="18.75">
@@ -2873,7 +2873,7 @@
       <c r="B93" s="11"/>
       <c r="C93" s="11"/>
       <c r="D93" s="11"/>
-      <c r="E93" s="32"/>
+      <c r="E93" s="23"/>
       <c r="F93" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="18.75">
@@ -2881,7 +2881,7 @@
       <c r="B94" s="11"/>
       <c r="C94" s="11"/>
       <c r="D94" s="11"/>
-      <c r="E94" s="32"/>
+      <c r="E94" s="23"/>
       <c r="F94" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="18.75">
@@ -2889,7 +2889,7 @@
       <c r="B95" s="11"/>
       <c r="C95" s="11"/>
       <c r="D95" s="11"/>
-      <c r="E95" s="32"/>
+      <c r="E95" s="23"/>
       <c r="F95" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="18.75">
@@ -2897,7 +2897,7 @@
       <c r="B96" s="11"/>
       <c r="C96" s="11"/>
       <c r="D96" s="11"/>
-      <c r="E96" s="32"/>
+      <c r="E96" s="23"/>
       <c r="F96" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="18.75">
@@ -2905,7 +2905,7 @@
       <c r="B97" s="11"/>
       <c r="C97" s="11"/>
       <c r="D97" s="11"/>
-      <c r="E97" s="32"/>
+      <c r="E97" s="23"/>
       <c r="F97" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="18.75">
@@ -2913,7 +2913,7 @@
       <c r="B98" s="11"/>
       <c r="C98" s="11"/>
       <c r="D98" s="11"/>
-      <c r="E98" s="32"/>
+      <c r="E98" s="23"/>
       <c r="F98" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="18.75">
@@ -2921,7 +2921,7 @@
       <c r="B99" s="11"/>
       <c r="C99" s="11"/>
       <c r="D99" s="11"/>
-      <c r="E99" s="32"/>
+      <c r="E99" s="23"/>
       <c r="F99" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="18.75">
@@ -2929,7 +2929,7 @@
       <c r="B100" s="11"/>
       <c r="C100" s="11"/>
       <c r="D100" s="11"/>
-      <c r="E100" s="32"/>
+      <c r="E100" s="23"/>
       <c r="F100" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="18.75">
@@ -2937,7 +2937,7 @@
       <c r="B101" s="11"/>
       <c r="C101" s="11"/>
       <c r="D101" s="11"/>
-      <c r="E101" s="32"/>
+      <c r="E101" s="23"/>
       <c r="F101" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="18.75">
@@ -2945,7 +2945,7 @@
       <c r="B102" s="11"/>
       <c r="C102" s="11"/>
       <c r="D102" s="11"/>
-      <c r="E102" s="32"/>
+      <c r="E102" s="23"/>
       <c r="F102" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="18.75">
@@ -2953,7 +2953,7 @@
       <c r="B103" s="11"/>
       <c r="C103" s="11"/>
       <c r="D103" s="11"/>
-      <c r="E103" s="32"/>
+      <c r="E103" s="23"/>
       <c r="F103" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="18.75">
@@ -2961,7 +2961,7 @@
       <c r="B104" s="11"/>
       <c r="C104" s="11"/>
       <c r="D104" s="11"/>
-      <c r="E104" s="32"/>
+      <c r="E104" s="23"/>
       <c r="F104" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="18.75">
@@ -2969,7 +2969,7 @@
       <c r="B105" s="11"/>
       <c r="C105" s="11"/>
       <c r="D105" s="11"/>
-      <c r="E105" s="32"/>
+      <c r="E105" s="23"/>
       <c r="F105" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="18.75">
@@ -2977,7 +2977,7 @@
       <c r="B106" s="11"/>
       <c r="C106" s="11"/>
       <c r="D106" s="11"/>
-      <c r="E106" s="32"/>
+      <c r="E106" s="23"/>
       <c r="F106" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="18.75">
@@ -2985,7 +2985,7 @@
       <c r="B107" s="11"/>
       <c r="C107" s="11"/>
       <c r="D107" s="11"/>
-      <c r="E107" s="32"/>
+      <c r="E107" s="23"/>
       <c r="F107" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="18.75">
@@ -2993,7 +2993,7 @@
       <c r="B108" s="11"/>
       <c r="C108" s="11"/>
       <c r="D108" s="11"/>
-      <c r="E108" s="32"/>
+      <c r="E108" s="23"/>
       <c r="F108" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="18.75">
@@ -6239,7 +6239,7 @@
       <c r="B9" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="31" t="s">
+      <c r="C9" s="32" t="s">
         <v>396</v>
       </c>
       <c r="D9" s="5" t="s">
@@ -6999,274 +6999,274 @@
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="24" t="s">
+      <c r="A1" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="26" t="s">
         <v>5</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="27" t="s">
         <v>353</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="28" t="s">
         <v>354</v>
       </c>
-      <c r="C2" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="27" t="s">
+      <c r="C2" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="28" t="s">
         <v>355</v>
       </c>
-      <c r="F2" s="28">
+      <c r="F2" s="29">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="27" t="s">
         <v>353</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="28" t="s">
         <v>356</v>
       </c>
-      <c r="C3" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="27" t="s">
+      <c r="C3" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="28" t="s">
         <v>357</v>
       </c>
-      <c r="F3" s="28">
+      <c r="F3" s="29">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="27" t="s">
         <v>353</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="28" t="s">
         <v>358</v>
       </c>
-      <c r="C4" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="27" t="s">
+      <c r="C4" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="28" t="s">
         <v>359</v>
       </c>
-      <c r="E4" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="29"/>
+      <c r="E4" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="30"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="27" t="s">
         <v>353</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="28" t="s">
         <v>360</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="D5" s="28" t="s">
         <v>361</v>
       </c>
-      <c r="E5" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="28">
+      <c r="E5" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="29">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="27" t="s">
         <v>353</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="28" t="s">
         <v>362</v>
       </c>
-      <c r="C6" s="27" t="s">
+      <c r="C6" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="D6" s="27" t="s">
+      <c r="D6" s="28" t="s">
         <v>363</v>
       </c>
-      <c r="E6" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="28">
+      <c r="E6" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="29">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="27" t="s">
         <v>353</v>
       </c>
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="28" t="s">
         <v>364</v>
       </c>
-      <c r="C7" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="27" t="s">
+      <c r="C7" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="28" t="s">
         <v>365</v>
       </c>
-      <c r="E7" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="29"/>
+      <c r="E7" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="30"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="27" t="s">
         <v>353</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="28" t="s">
         <v>366</v>
       </c>
-      <c r="C8" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="27" t="s">
+      <c r="C8" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="28" t="s">
         <v>367</v>
       </c>
-      <c r="E8" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" s="29"/>
+      <c r="E8" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="30"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="26" t="s">
+      <c r="A9" s="27" t="s">
         <v>353</v>
       </c>
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="28" t="s">
         <v>368</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="D9" s="27" t="s">
+      <c r="D9" s="28" t="s">
         <v>369</v>
       </c>
-      <c r="E9" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" s="28">
+      <c r="E9" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="29">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
-      <c r="A10" s="26" t="s">
+      <c r="A10" s="27" t="s">
         <v>353</v>
       </c>
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="28" t="s">
         <v>370</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="C10" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="D10" s="27" t="s">
+      <c r="D10" s="28" t="s">
         <v>371</v>
       </c>
-      <c r="E10" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" s="28">
+      <c r="E10" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="29">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
-      <c r="A11" s="26" t="s">
+      <c r="A11" s="27" t="s">
         <v>353</v>
       </c>
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="28" t="s">
         <v>372</v>
       </c>
-      <c r="C11" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="27" t="s">
+      <c r="C11" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="28" t="s">
         <v>373</v>
       </c>
-      <c r="E11" s="27" t="s">
+      <c r="E11" s="28" t="s">
         <v>374</v>
       </c>
-      <c r="F11" s="28">
+      <c r="F11" s="29">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
-      <c r="A12" s="26" t="s">
+      <c r="A12" s="27" t="s">
         <v>353</v>
       </c>
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="28" t="s">
         <v>375</v>
       </c>
-      <c r="C12" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="27" t="s">
+      <c r="C12" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="28" t="s">
         <v>373</v>
       </c>
-      <c r="E12" s="27" t="s">
+      <c r="E12" s="28" t="s">
         <v>376</v>
       </c>
-      <c r="F12" s="28">
+      <c r="F12" s="29">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
-      <c r="A13" s="26" t="s">
+      <c r="A13" s="27" t="s">
         <v>353</v>
       </c>
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="28" t="s">
         <v>377</v>
       </c>
-      <c r="C13" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="27" t="s">
+      <c r="C13" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="28" t="s">
         <v>378</v>
       </c>
-      <c r="E13" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="F13" s="29"/>
+      <c r="E13" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="30"/>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
-      <c r="A14" s="26" t="s">
+      <c r="A14" s="27" t="s">
         <v>353</v>
       </c>
-      <c r="B14" s="26" t="s">
+      <c r="B14" s="27" t="s">
         <v>379</v>
       </c>
-      <c r="C14" s="26" t="s">
+      <c r="C14" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="D14" s="26" t="s">
+      <c r="D14" s="27" t="s">
         <v>380</v>
       </c>
-      <c r="E14" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="F14" s="30">
+      <c r="E14" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="31">
         <v>0</v>
       </c>
     </row>
@@ -7892,7 +7892,7 @@
       <c r="L23" s="11"/>
       <c r="M23" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="11" t="s">
         <v>263</v>
       </c>
@@ -7917,7 +7917,7 @@
       <c r="L24" s="11"/>
       <c r="M24" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="11" t="s">
         <v>263</v>
       </c>
@@ -7942,7 +7942,7 @@
       <c r="L25" s="11"/>
       <c r="M25" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
       <c r="A26" s="11" t="s">
         <v>263</v>
       </c>
@@ -7969,7 +7969,7 @@
       <c r="L26" s="11"/>
       <c r="M26" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
       <c r="A27" s="11" t="s">
         <v>263</v>
       </c>
@@ -7994,7 +7994,7 @@
       <c r="L27" s="11"/>
       <c r="M27" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
       <c r="A28" s="11" t="s">
         <v>263</v>
       </c>
@@ -8019,7 +8019,7 @@
       <c r="L28" s="11"/>
       <c r="M28" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
       <c r="A29" s="11" t="s">
         <v>263</v>
       </c>
@@ -8044,7 +8044,7 @@
       <c r="L29" s="11"/>
       <c r="M29" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
       <c r="A30" s="11" t="s">
         <v>263</v>
       </c>
@@ -8069,7 +8069,7 @@
       <c r="L30" s="11"/>
       <c r="M30" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
       <c r="A31" s="11" t="s">
         <v>263</v>
       </c>
@@ -8094,7 +8094,7 @@
       <c r="L31" s="11"/>
       <c r="M31" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
       <c r="A32" s="11" t="s">
         <v>263</v>
       </c>
@@ -8865,7 +8865,7 @@
       <c r="C4" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="23" t="s">
         <v>72</v>
       </c>
       <c r="E4" s="11" t="s">

</xml_diff>